<commit_message>
Documentção e padrõnização código
</commit_message>
<xml_diff>
--- a/modelos.xlsx
+++ b/modelos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\osmar\Documentos\GitHub\texto-transformer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B84794F-8EA6-42F5-8131-9F6F24F58CC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B0383D3-9B72-407A-B61B-46C68983DA24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="15375" windowHeight="7875" xr2:uid="{ADA84CBB-E06D-42EE-8062-4654A38564A2}"/>
+    <workbookView xWindow="3285" yWindow="2070" windowWidth="15375" windowHeight="7875" xr2:uid="{ADA84CBB-E06D-42EE-8062-4654A38564A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>modelo</t>
   </si>
@@ -44,9 +44,6 @@
     <t>BERT</t>
   </si>
   <si>
-    <t>CLS,SEP,UNK</t>
-  </si>
-  <si>
     <t>Albert</t>
   </si>
   <si>
@@ -92,13 +89,31 @@
     <t>['I', 'play', 'bass', 'in', 'a', 'jazz', 'band', '.']</t>
   </si>
   <si>
-    <t>CLS,SEP,&lt;unk&gt;</t>
-  </si>
-  <si>
     <t>lower_case</t>
   </si>
   <si>
     <t>ROBERTa</t>
+  </si>
+  <si>
+    <t>&lt;s&gt;&lt;pad&gt;&lt;/s&gt;&lt;unk&gt;&lt;mask&gt;</t>
+  </si>
+  <si>
+    <t>CLS,SEP,MASK, PAD, UNK</t>
+  </si>
+  <si>
+    <t>CLS,SEP,MASK, PAD, &lt;unk&gt;</t>
+  </si>
+  <si>
+    <t>algoritmo</t>
+  </si>
+  <si>
+    <t>Wordpice</t>
+  </si>
+  <si>
+    <t>SentencePiece</t>
+  </si>
+  <si>
+    <t xml:space="preserve">byte-pair-encoding (BPE) [ Sennrich et al. ] </t>
   </si>
 </sst>
 </file>
@@ -462,7 +477,7 @@
   <dimension ref="A2:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,19 +492,22 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
         <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -497,64 +515,79 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="G3" t="s">
+        <v>23</v>
       </c>
       <c r="I3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>24</v>
       </c>
       <c r="I4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="G5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" t="s">
         <v>16</v>
-      </c>
-      <c r="I5" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="G6" t="s">
+        <v>25</v>
       </c>
       <c r="I6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Organização do código fonte.
</commit_message>
<xml_diff>
--- a/modelos.xlsx
+++ b/modelos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\osmar\Documentos\GitHub\texto-transformer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{395E1239-8A2E-41AC-9FE5-4ECBAD17B865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A56212FA-8D14-499B-A68B-15F1DBCB4FF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3285" yWindow="2070" windowWidth="15375" windowHeight="7875" xr2:uid="{ADA84CBB-E06D-42EE-8062-4654A38564A2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{ADA84CBB-E06D-42EE-8062-4654A38564A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -89,9 +89,6 @@
     <t>lower_case</t>
   </si>
   <si>
-    <t>ROBERTa</t>
-  </si>
-  <si>
     <t>&lt;s&gt;&lt;pad&gt;&lt;/s&gt;&lt;unk&gt;&lt;mask&gt;</t>
   </si>
   <si>
@@ -129,6 +126,9 @@
   </si>
   <si>
     <t>[UNK]</t>
+  </si>
+  <si>
+    <t>RoBERTa</t>
   </si>
 </sst>
 </file>
@@ -489,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D3D3DC9-8A8A-4ECE-AF2B-5AE8D9558D5B}">
-  <dimension ref="A2:I6"/>
+  <dimension ref="A2:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,16 +515,16 @@
         <v>11</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I2" t="s">
         <v>7</v>
@@ -535,7 +535,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
@@ -544,10 +544,10 @@
         <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I3" t="s">
         <v>3</v>
@@ -558,7 +558,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
@@ -567,13 +567,13 @@
         <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F4" t="s">
         <v>12</v>
       </c>
       <c r="G4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I4" t="s">
         <v>5</v>
@@ -584,16 +584,16 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
         <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I5" t="s">
         <v>15</v>
@@ -601,10 +601,10 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" t="s">
         <v>17</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
@@ -613,14 +613,17 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I6" t="s">
         <v>4</v>
       </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -629,6 +632,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100886399F21440F54B81A4893F74DA4F94" ma:contentTypeVersion="8" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="91b6ab92f34ab688a19900d483ae7505">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0190bee1-42b9-4362-9dc8-2229f310bd34" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d4f82e64d1772ab8a19658e1978de7e8" ns3:_="">
     <xsd:import namespace="0190bee1-42b9-4362-9dc8-2229f310bd34"/>
@@ -798,15 +810,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -814,6 +817,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6C04E1C-86C9-4DFF-AFD3-8243B20410CC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FBDDB8E-E50B-4DEA-B8C8-CD7F650AB124}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -831,14 +842,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6C04E1C-86C9-4DFF-AFD3-8243B20410CC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38DEF460-956D-41C9-BA67-8231780B003F}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Testes unitários do XLNet
</commit_message>
<xml_diff>
--- a/modelos.xlsx
+++ b/modelos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\osmar\Documentos\GitHub\texto-transformer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A56212FA-8D14-499B-A68B-15F1DBCB4FF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{880289BB-DF1E-4580-8E45-2E42879B5E8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{ADA84CBB-E06D-42EE-8062-4654A38564A2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="56">
   <si>
     <t>modelo</t>
   </si>
@@ -47,18 +47,6 @@
     <t>Albert</t>
   </si>
   <si>
-    <t>['Ado', '##ro', 'sor', '##vete', 'de', 'mang', '##a', '.']</t>
-  </si>
-  <si>
-    <t>['Su', 'je', 'i', 'Ġa', 'Ġmanga', 'Ġda', 'Ġcam', 'isa', '.']</t>
-  </si>
-  <si>
-    <t>['▁a', 'doro', '▁sor', 've', 'te', '▁de', '▁manga', '.']</t>
-  </si>
-  <si>
-    <t>tokens especiais</t>
-  </si>
-  <si>
     <t>Exemplo</t>
   </si>
   <si>
@@ -83,21 +71,9 @@
     <t>false</t>
   </si>
   <si>
-    <t>['I', 'play', 'bass', 'in', 'a', 'jazz', 'band', '.']</t>
-  </si>
-  <si>
     <t>lower_case</t>
   </si>
   <si>
-    <t>&lt;s&gt;&lt;pad&gt;&lt;/s&gt;&lt;unk&gt;&lt;mask&gt;</t>
-  </si>
-  <si>
-    <t>CLS,SEP,MASK, PAD, UNK</t>
-  </si>
-  <si>
-    <t>CLS,SEP,MASK, PAD, &lt;unk&gt;</t>
-  </si>
-  <si>
     <t>algoritmo</t>
   </si>
   <si>
@@ -116,9 +92,6 @@
     <t>subtoken</t>
   </si>
   <si>
-    <t>subtoken desconhecido</t>
-  </si>
-  <si>
     <t>Â</t>
   </si>
   <si>
@@ -129,13 +102,115 @@
   </si>
   <si>
     <t>RoBERTa</t>
+  </si>
+  <si>
+    <t>XLNet</t>
+  </si>
+  <si>
+    <t>['&lt;s&gt;','Su', 'je', 'i', 'Ġa', 'Ġmanga', 'Ġda', 'Ġcam', 'isa', '.','&lt;/s&gt;]</t>
+  </si>
+  <si>
+    <t>['[CLS]','Ado', '##ro', 'sor', '##vete', 'de', 'mang', '##a', '.', '[SEP]']</t>
+  </si>
+  <si>
+    <t>['[CLS]','▁a', 'doro', '▁sor', 've', 'te', '▁de', '▁manga', '.','[SEP]']</t>
+  </si>
+  <si>
+    <t>['[CLS]','I', 'play', 'bass', 'in', 'a', 'jazz', 'band', '.','[SEP]']</t>
+  </si>
+  <si>
+    <t>['▁a', 'doro', '▁sor', 've', 'te', '▁de', '▁manga', '.','&lt;sep&gt;','&lt;cls&gt;']</t>
+  </si>
+  <si>
+    <t>pad_token</t>
+  </si>
+  <si>
+    <t>[PAD]</t>
+  </si>
+  <si>
+    <t>&lt;pad&gt;</t>
+  </si>
+  <si>
+    <t>mask_token</t>
+  </si>
+  <si>
+    <t>[MASK]</t>
+  </si>
+  <si>
+    <t>&lt;mask&gt;</t>
+  </si>
+  <si>
+    <t>eos_token</t>
+  </si>
+  <si>
+    <t>bos_token</t>
+  </si>
+  <si>
+    <t>cls_token</t>
+  </si>
+  <si>
+    <t>[CLS]</t>
+  </si>
+  <si>
+    <t>&lt;cls&gt;</t>
+  </si>
+  <si>
+    <t>&lt;s&gt;</t>
+  </si>
+  <si>
+    <t>unk_token</t>
+  </si>
+  <si>
+    <t>&lt;/s&gt;</t>
+  </si>
+  <si>
+    <t>[SEP]</t>
+  </si>
+  <si>
+    <t>sep_token</t>
+  </si>
+  <si>
+    <t>&lt;sep&gt;</t>
+  </si>
+  <si>
+    <t>sentença simples</t>
+  </si>
+  <si>
+    <t>par de sentenças</t>
+  </si>
+  <si>
+    <t>&lt;s&gt; X &lt;/s&gt;</t>
+  </si>
+  <si>
+    <t>&lt;s&gt; A &lt;/s&gt;&lt;/s&gt; B &lt;/s&gt;</t>
+  </si>
+  <si>
+    <t>[CLS] X [SEP]</t>
+  </si>
+  <si>
+    <t>[CLS] A [SEP] B [SEP]</t>
+  </si>
+  <si>
+    <t>X &lt;sep&gt; &lt;cls&gt;</t>
+  </si>
+  <si>
+    <t>A &lt;sep&gt; B &lt;sep&gt; &lt;cls&gt;</t>
+  </si>
+  <si>
+    <t>padding_side</t>
+  </si>
+  <si>
+    <t>direita</t>
+  </si>
+  <si>
+    <t>esquerda</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,6 +221,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -172,9 +255,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -489,141 +573,313 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D3D3DC9-8A8A-4ECE-AF2B-5AE8D9558D5B}">
-  <dimension ref="A2:I7"/>
+  <dimension ref="A2:P7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="5.28515625" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" customWidth="1"/>
+    <col min="5" max="5" width="7" customWidth="1"/>
+    <col min="6" max="7" width="7.42578125" customWidth="1"/>
+    <col min="8" max="8" width="8" customWidth="1"/>
+    <col min="9" max="9" width="7.5703125" customWidth="1"/>
+    <col min="10" max="10" width="8.140625" customWidth="1"/>
+    <col min="11" max="11" width="5.5703125" customWidth="1"/>
+    <col min="12" max="12" width="6.140625" customWidth="1"/>
+    <col min="14" max="14" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" t="s">
-        <v>7</v>
+      <c r="M2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="D3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="K3" t="s">
+        <v>4</v>
+      </c>
+      <c r="M3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N3" t="s">
+        <v>49</v>
+      </c>
+      <c r="O3" t="s">
+        <v>50</v>
+      </c>
+      <c r="P3" t="s">
         <v>24</v>
       </c>
-      <c r="I3" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" t="s">
         <v>19</v>
       </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="J4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K4" t="s">
+        <v>5</v>
+      </c>
+      <c r="L4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M4" t="s">
+        <v>14</v>
+      </c>
+      <c r="N4" t="s">
+        <v>49</v>
+      </c>
+      <c r="O4" t="s">
+        <v>50</v>
+      </c>
+      <c r="P4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" t="s">
+        <v>10</v>
+      </c>
+      <c r="M5" t="s">
+        <v>13</v>
+      </c>
+      <c r="N5" t="s">
+        <v>47</v>
+      </c>
+      <c r="O5" t="s">
+        <v>48</v>
+      </c>
+      <c r="P5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" t="s">
+        <v>8</v>
+      </c>
+      <c r="K6" t="s">
+        <v>6</v>
+      </c>
+      <c r="M6" t="s">
+        <v>15</v>
+      </c>
+      <c r="N6" t="s">
+        <v>49</v>
+      </c>
+      <c r="O6" t="s">
+        <v>50</v>
+      </c>
+      <c r="P6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I4" t="s">
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="M7" t="s">
         <v>14</v>
       </c>
-      <c r="E5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5" t="s">
-        <v>21</v>
-      </c>
-      <c r="I5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="N7" t="s">
+        <v>51</v>
+      </c>
+      <c r="O7" t="s">
+        <v>52</v>
+      </c>
+      <c r="P7" t="s">
         <v>27</v>
       </c>
-      <c r="G6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Configuração e testes OpenAIGPT
</commit_message>
<xml_diff>
--- a/modelos.xlsx
+++ b/modelos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\osmar\Documentos\GitHub\texto-transformer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB8282F-AB49-4082-93DC-FEBCC46A1440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DC0E46E-F986-43E5-B3F1-149D16CF04FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{ADA84CBB-E06D-42EE-8062-4654A38564A2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="87">
   <si>
     <t>modelo</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Ġ</t>
   </si>
   <si>
-    <t>subtokens</t>
-  </si>
-  <si>
     <t>true</t>
   </si>
   <si>
@@ -107,18 +104,6 @@
     <t>XLNet</t>
   </si>
   <si>
-    <t>['[CLS]','Ado', '##ro', 'sor', '##vete', 'de', 'mang', '##a', '.', '[SEP]']</t>
-  </si>
-  <si>
-    <t>['[CLS]','▁a', 'doro', '▁sor', 've', 'te', '▁de', '▁manga', '.','[SEP]']</t>
-  </si>
-  <si>
-    <t>['[CLS]','I', 'play', 'bass', 'in', 'a', 'jazz', 'band', '.','[SEP]']</t>
-  </si>
-  <si>
-    <t>['▁a', 'doro', '▁sor', 've', 'te', '▁de', '▁manga', '.','&lt;sep&gt;','&lt;cls&gt;']</t>
-  </si>
-  <si>
     <t>pad_token</t>
   </si>
   <si>
@@ -197,12 +182,6 @@
     <t>padding_side</t>
   </si>
   <si>
-    <t>direita</t>
-  </si>
-  <si>
-    <t>esquerda</t>
-  </si>
-  <si>
     <t>GPT-2</t>
   </si>
   <si>
@@ -215,17 +194,116 @@
     <t>A , B</t>
   </si>
   <si>
-    <t>['Su', 'je', 'i', 'Ġa', 'Ġmanga', 'Ġda', 'Ġcam', 'isa', '.']</t>
-  </si>
-  <si>
-    <t>['&lt;s&gt;','Su', 'je', 'i', 'Ġa', 'Ġmanga', 'Ġda', 'Ġcam', 'isa', '.','&lt;/s&gt;']</t>
+    <t>OpenAIGPTModel</t>
+  </si>
+  <si>
+    <t>&lt;/w&gt;</t>
+  </si>
+  <si>
+    <t>['[CLS]', 'Fresh', 'sea', 'bass', 'is', 'a', 'great', 'del', '##ica', '##cy', '.', '[SEP]']</t>
+  </si>
+  <si>
+    <t>['Fresh', 'Ġsea', 'Ġbass', 'Ġis', 'Ġa', 'Ġgreat', 'Ġdelic', 'acy', '.']</t>
+  </si>
+  <si>
+    <t>['[CLS]', '▁fresh', '▁sea', '▁bass', '▁is', '▁a', '▁great', '▁', 'delic', 'acy', '.', '[SEP]']</t>
+  </si>
+  <si>
+    <t>['▁Fresh', '▁sea', '▁bass', '▁is', '▁a', '▁great', '▁de', 'lic', 'acy', '.', '&lt;sep&gt;', '&lt;cls&gt;']</t>
+  </si>
+  <si>
+    <t>['fresh&lt;/w&gt;', 'sea&lt;/w&gt;', 'bass&lt;/w&gt;', 'is&lt;/w&gt;', 'a&lt;/w&gt;', 'great&lt;/w&gt;', 'deli', 'ca', 'cy&lt;/w&gt;', '.&lt;/w&gt;']</t>
+  </si>
+  <si>
+    <t>início</t>
+  </si>
+  <si>
+    <t>fim</t>
+  </si>
+  <si>
+    <t>sem subtoken</t>
+  </si>
+  <si>
+    <t>separador_subtoken</t>
+  </si>
+  <si>
+    <t>separador_subtoken_position</t>
+  </si>
+  <si>
+    <t>separador_subtoken_repetition</t>
+  </si>
+  <si>
+    <t>nos subtokens(menos primeiro)</t>
+  </si>
+  <si>
+    <t>['&lt;s&gt;', 'Fresh', 'Ġsea', 'Ġbass', 'Ġis', 'Ġa', 'Ġgreat', 'Ġdelic', 'acy', 'Ġ.', '&lt;/s&gt;']</t>
+  </si>
+  <si>
+    <t>somente primeiro subtoken</t>
+  </si>
+  <si>
+    <t>somente último subtoken</t>
+  </si>
+  <si>
+    <t>https://github.com/huggingface/transformers/blob/v4.30.0/src/transformers/models/gpt2/tokenization_gpt2.py</t>
+  </si>
+  <si>
+    <t>Documentação</t>
+  </si>
+  <si>
+    <t>https://github.com/huggingface/transformers/blob/v4.30.0/src/transformers/models/openai/tokenization_openai.py</t>
+  </si>
+  <si>
+    <t>https://github.com/huggingface/transformers/blob/v4.30.0/src/transformers/models/xlnet/tokenization_xlnet.py</t>
+  </si>
+  <si>
+    <t>https://github.com/huggingface/transformers/blob/v4.30.0/src/transformers/models/roberta/tokenization_roberta.py</t>
+  </si>
+  <si>
+    <t>https://github.com/huggingface/transformers/blob/v4.30.0/src/transformers/models/distilbert/tokenization_distilbert.py</t>
+  </si>
+  <si>
+    <t>https://github.com/huggingface/transformers/blob/v4.30.0/src/transformers/models/albert/tokenization_albert.py</t>
+  </si>
+  <si>
+    <t>https://github.com/huggingface/transformers/blob/v4.30.0/src/transformers/models/bert/tokenization_bert.py</t>
+  </si>
+  <si>
+    <t>Código fonte</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/docs/transformers/model_doc/bert#transformers.BertTokenizer</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/docs/transformers/model_doc/albert#transformers.AlbertTokenizer</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/docs/transformers/model_doc/distilbert#transformers.DistilBertTokenizer</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/docs/transformers/model_doc/roberta#transformers.RobertaTokenizer</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/docs/transformers/model_doc/xlnet#transformers.XLNetTokenizer</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/docs/transformers/model_doc/gpt2#transformers.GPT2Tokenizer</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/docs/transformers/model_doc/openai-gpt#transformers.OpenAIGPTTokenizer</t>
+  </si>
+  <si>
+    <t>0 esquerda</t>
+  </si>
+  <si>
+    <t>1 direita</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -249,6 +327,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -267,15 +353,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -588,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D3D3DC9-8A8A-4ECE-AF2B-5AE8D9558D5B}">
-  <dimension ref="A2:P8"/>
+  <dimension ref="A2:AB20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,355 +690,581 @@
     <col min="2" max="2" width="5.28515625" customWidth="1"/>
     <col min="3" max="3" width="5.7109375" customWidth="1"/>
     <col min="4" max="4" width="6.140625" customWidth="1"/>
-    <col min="5" max="5" width="7" customWidth="1"/>
-    <col min="6" max="7" width="7.42578125" customWidth="1"/>
+    <col min="5" max="5" width="5.140625" customWidth="1"/>
+    <col min="6" max="6" width="6" customWidth="1"/>
+    <col min="7" max="7" width="6.140625" customWidth="1"/>
     <col min="8" max="8" width="8" customWidth="1"/>
     <col min="9" max="9" width="7.5703125" customWidth="1"/>
     <col min="10" max="10" width="7.140625" customWidth="1"/>
-    <col min="11" max="11" width="5.5703125" customWidth="1"/>
-    <col min="12" max="12" width="6.140625" customWidth="1"/>
-    <col min="14" max="14" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="5.5703125" customWidth="1"/>
+    <col min="14" max="14" width="6.140625" customWidth="1"/>
+    <col min="16" max="16" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="P2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="P2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="R2" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="AA2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>77</v>
+      </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
         <v>36</v>
       </c>
-      <c r="C3" t="s">
-        <v>41</v>
-      </c>
       <c r="D3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="F3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" t="s">
-        <v>53</v>
+        <v>23</v>
+      </c>
+      <c r="G3" s="3">
+        <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="I3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K3" t="s">
         <v>4</v>
       </c>
-      <c r="M3" t="s">
-        <v>16</v>
-      </c>
-      <c r="N3" t="s">
-        <v>48</v>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
       </c>
       <c r="O3" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="P3" t="s">
-        <v>23</v>
+        <v>43</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>44</v>
+      </c>
+      <c r="R3" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA3" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB3" s="4" t="s">
+        <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
         <v>36</v>
       </c>
-      <c r="C4" t="s">
-        <v>41</v>
-      </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="F4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" t="s">
-        <v>53</v>
+        <v>24</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="I4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K4" t="s">
         <v>5</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4" t="s">
+        <v>7</v>
+      </c>
+      <c r="O4" t="s">
+        <v>13</v>
+      </c>
+      <c r="P4" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>44</v>
+      </c>
+      <c r="R4" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA4" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB4" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M4" t="s">
-        <v>14</v>
-      </c>
-      <c r="N4" t="s">
-        <v>48</v>
-      </c>
-      <c r="O4" t="s">
-        <v>49</v>
-      </c>
-      <c r="P4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" t="s">
         <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" t="s">
-        <v>53</v>
-      </c>
-      <c r="H5" t="s">
-        <v>31</v>
-      </c>
-      <c r="I5" t="s">
-        <v>20</v>
-      </c>
-      <c r="J5" t="s">
-        <v>10</v>
       </c>
       <c r="K5" t="s">
         <v>4</v>
       </c>
-      <c r="M5" t="s">
-        <v>13</v>
-      </c>
-      <c r="N5" t="s">
-        <v>48</v>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
       </c>
       <c r="O5" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="P5" t="s">
-        <v>25</v>
+        <v>43</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>44</v>
+      </c>
+      <c r="R5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA5" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB5" s="4" t="s">
+        <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D6" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E6" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="F6" t="s">
-        <v>29</v>
-      </c>
-      <c r="G6" t="s">
-        <v>53</v>
+        <v>24</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
       </c>
       <c r="H6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="I6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K6" t="s">
         <v>6</v>
       </c>
-      <c r="M6" t="s">
-        <v>15</v>
-      </c>
-      <c r="N6" t="s">
-        <v>46</v>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
       </c>
       <c r="O6" t="s">
-        <v>47</v>
+        <v>14</v>
       </c>
       <c r="P6" t="s">
-        <v>60</v>
+        <v>41</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>42</v>
+      </c>
+      <c r="R6" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA6" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AB6" s="4" t="s">
+        <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" t="s">
         <v>38</v>
       </c>
-      <c r="C7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" t="s">
-        <v>43</v>
-      </c>
       <c r="E7" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="F7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G7" t="s">
-        <v>54</v>
+        <v>24</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
       </c>
       <c r="H7" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="I7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K7" t="s">
         <v>5</v>
       </c>
-      <c r="M7" t="s">
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="O7" t="s">
+        <v>13</v>
+      </c>
+      <c r="P7" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>46</v>
+      </c>
+      <c r="R7" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA7" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB7" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8" t="s">
+        <v>49</v>
+      </c>
+      <c r="I8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" t="s">
+        <v>7</v>
+      </c>
+      <c r="K8" t="s">
+        <v>53</v>
+      </c>
+      <c r="L8">
+        <v>2</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8" t="s">
+        <v>7</v>
+      </c>
+      <c r="O8" t="s">
         <v>14</v>
       </c>
-      <c r="N7" t="s">
+      <c r="P8" t="s">
         <v>50</v>
       </c>
-      <c r="O7" t="s">
+      <c r="Q8" t="s">
         <v>51</v>
       </c>
-      <c r="P7" t="s">
-        <v>26</v>
+      <c r="R8" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA8" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="AB8" s="4" t="s">
+        <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I9" t="s">
+        <v>49</v>
+      </c>
+      <c r="J9" t="s">
+        <v>7</v>
+      </c>
+      <c r="K9" t="s">
+        <v>6</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="O9" t="s">
+        <v>14</v>
+      </c>
+      <c r="P9" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>51</v>
+      </c>
+      <c r="R9" t="s">
         <v>55</v>
       </c>
-      <c r="B8" t="s">
-        <v>56</v>
-      </c>
-      <c r="C8" t="s">
-        <v>56</v>
-      </c>
-      <c r="D8" t="s">
-        <v>56</v>
-      </c>
-      <c r="E8" t="s">
-        <v>56</v>
-      </c>
-      <c r="F8" t="s">
-        <v>28</v>
-      </c>
-      <c r="G8" t="s">
-        <v>53</v>
-      </c>
-      <c r="H8" t="s">
-        <v>56</v>
-      </c>
-      <c r="I8" t="s">
-        <v>56</v>
-      </c>
-      <c r="J8" t="s">
-        <v>8</v>
-      </c>
-      <c r="K8" t="s">
-        <v>6</v>
-      </c>
-      <c r="M8" t="s">
-        <v>15</v>
-      </c>
-      <c r="N8" t="s">
-        <v>57</v>
-      </c>
-      <c r="O8" t="s">
-        <v>58</v>
-      </c>
-      <c r="P8" t="s">
+      <c r="AA9" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB9" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>85</v>
+      </c>
+      <c r="L12">
+        <v>-1</v>
+      </c>
+      <c r="M12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="G13" t="s">
+        <v>86</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="L15">
+        <v>2</v>
+      </c>
+      <c r="M15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M18">
+        <v>-1</v>
+      </c>
+      <c r="N18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19" t="s">
         <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M20">
+        <v>1</v>
+      </c>
+      <c r="N20" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="AA3" r:id="rId1" location="transformers.BertTokenizer" xr:uid="{34D2F53E-DD38-4D02-B9D7-EEB3C73565A4}"/>
+    <hyperlink ref="AA4" r:id="rId2" location="transformers.AlbertTokenizer" xr:uid="{1C747986-9A2C-4D37-85D4-551E037E79AF}"/>
+    <hyperlink ref="AA5" r:id="rId3" location="transformers.DistilBertTokenizer" xr:uid="{4557F4E1-3CF5-452D-B493-FBA68FEF70C1}"/>
+    <hyperlink ref="AA6" r:id="rId4" location="transformers.RobertaTokenizer" xr:uid="{38642F05-9C73-4563-BF96-AEE8C072DC8E}"/>
+    <hyperlink ref="AA7" r:id="rId5" location="transformers.XLNetTokenizer" xr:uid="{287DC99E-D4A0-4091-81B9-FD3CC7A6D5AB}"/>
+    <hyperlink ref="AA8" r:id="rId6" location="transformers.OpenAIGPTTokenizer" xr:uid="{1381AF7A-FED8-43A8-B952-743B3E821ABF}"/>
+    <hyperlink ref="AA9" r:id="rId7" location="transformers.GPT2Tokenizer" xr:uid="{D91A5263-1AFB-40F8-BF67-C0F7CF6DD3B8}"/>
+    <hyperlink ref="AB3" r:id="rId8" xr:uid="{5ED3647C-C8FA-443D-AAEB-9454BBCF6176}"/>
+    <hyperlink ref="AB4" r:id="rId9" xr:uid="{118612AF-F178-449D-94F5-EA8FCCE6B629}"/>
+    <hyperlink ref="AB5" r:id="rId10" xr:uid="{9F819B38-1C37-4436-86A4-26447E432B97}"/>
+    <hyperlink ref="AB6" r:id="rId11" xr:uid="{3E18BD0A-C819-47DD-AF95-3DFEF2DEB3D5}"/>
+    <hyperlink ref="AB7" r:id="rId12" xr:uid="{E2C80B92-5270-44E6-BA42-98A672C126C8}"/>
+    <hyperlink ref="AB8" r:id="rId13" xr:uid="{65DBFE01-0236-40D1-BAA2-DBC7A7D06BBE}"/>
+    <hyperlink ref="AB9" r:id="rId14" xr:uid="{31303705-0E07-4F0C-A889-CB48F2A8D49E}"/>
+  </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId15"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Formatação do código em tokenização palavra.
</commit_message>
<xml_diff>
--- a/modelos.xlsx
+++ b/modelos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\osmar\Documentos\GitHub\texto-transformer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DC0E46E-F986-43E5-B3F1-149D16CF04FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF5E33D-89F2-49DE-96B4-354B4D5AD052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{ADA84CBB-E06D-42EE-8062-4654A38564A2}"/>
   </bookViews>
@@ -680,8 +680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D3D3DC9-8A8A-4ECE-AF2B-5AE8D9558D5B}">
   <dimension ref="A2:AB20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -689,7 +689,7 @@
     <col min="1" max="1" width="9.5703125" customWidth="1"/>
     <col min="2" max="2" width="5.28515625" customWidth="1"/>
     <col min="3" max="3" width="5.7109375" customWidth="1"/>
-    <col min="4" max="4" width="6.140625" customWidth="1"/>
+    <col min="4" max="4" width="5.85546875" customWidth="1"/>
     <col min="5" max="5" width="5.140625" customWidth="1"/>
     <col min="6" max="6" width="6" customWidth="1"/>
     <col min="7" max="7" width="6.140625" customWidth="1"/>
@@ -698,7 +698,7 @@
     <col min="10" max="10" width="7.140625" customWidth="1"/>
     <col min="11" max="13" width="5.5703125" customWidth="1"/>
     <col min="14" max="14" width="6.140625" customWidth="1"/>
-    <col min="16" max="16" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13" customWidth="1"/>
     <col min="17" max="17" width="20" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1269,15 +1269,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100886399F21440F54B81A4893F74DA4F94" ma:contentTypeVersion="8" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="91b6ab92f34ab688a19900d483ae7505">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0190bee1-42b9-4362-9dc8-2229f310bd34" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d4f82e64d1772ab8a19658e1978de7e8" ns3:_="">
     <xsd:import namespace="0190bee1-42b9-4362-9dc8-2229f310bd34"/>
@@ -1447,6 +1438,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1454,14 +1454,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6C04E1C-86C9-4DFF-AFD3-8243B20410CC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FBDDB8E-E50B-4DEA-B8C8-CD7F650AB124}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1475,6 +1467,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6C04E1C-86C9-4DFF-AFD3-8243B20410CC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Factory Method para Transformer.
</commit_message>
<xml_diff>
--- a/modelos.xlsx
+++ b/modelos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\osmar\Documentos\GitHub\texto-transformer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF5E33D-89F2-49DE-96B4-354B4D5AD052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{968172B3-96E2-4178-A4D1-9D3F137C9D75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{ADA84CBB-E06D-42EE-8062-4654A38564A2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="90">
   <si>
     <t>modelo</t>
   </si>
@@ -230,9 +230,6 @@
     <t>separador_subtoken_position</t>
   </si>
   <si>
-    <t>separador_subtoken_repetition</t>
-  </si>
-  <si>
     <t>nos subtokens(menos primeiro)</t>
   </si>
   <si>
@@ -293,17 +290,29 @@
     <t>https://huggingface.co/docs/transformers/model_doc/openai-gpt#transformers.OpenAIGPTTokenizer</t>
   </si>
   <si>
-    <t>0 esquerda</t>
-  </si>
-  <si>
-    <t>1 direita</t>
+    <t>separador_subtoken_repeticao</t>
+  </si>
+  <si>
+    <t>primeiro_token_sem_separador</t>
+  </si>
+  <si>
+    <t>posicao_token_final</t>
+  </si>
+  <si>
+    <t>posicao_token_inicio</t>
+  </si>
+  <si>
+    <t>preenchimento pad a esquerda</t>
+  </si>
+  <si>
+    <t>preenchimento pad a direita</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -335,6 +344,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -357,12 +375,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -678,10 +697,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D3D3DC9-8A8A-4ECE-AF2B-5AE8D9558D5B}">
-  <dimension ref="A2:AB20"/>
+  <dimension ref="A2:AE20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,14 +715,14 @@
     <col min="8" max="8" width="8" customWidth="1"/>
     <col min="9" max="9" width="7.5703125" customWidth="1"/>
     <col min="10" max="10" width="7.140625" customWidth="1"/>
-    <col min="11" max="13" width="5.5703125" customWidth="1"/>
-    <col min="14" max="14" width="6.140625" customWidth="1"/>
-    <col min="16" max="16" width="13" customWidth="1"/>
-    <col min="17" max="17" width="20" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="16" width="5.5703125" customWidth="1"/>
+    <col min="17" max="17" width="6.140625" customWidth="1"/>
+    <col min="19" max="19" width="13" customWidth="1"/>
+    <col min="20" max="20" width="20" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -738,34 +757,43 @@
         <v>62</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="M2" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="P2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="AA2" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="AB2" s="1" t="s">
-        <v>77</v>
+      <c r="AD2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -800,31 +828,43 @@
         <v>4</v>
       </c>
       <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>-1</v>
+      </c>
+      <c r="N3">
         <v>0</v>
       </c>
-      <c r="M3">
+      <c r="O3">
         <v>0</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>9</v>
+      </c>
+      <c r="R3" t="s">
         <v>15</v>
       </c>
-      <c r="P3" t="s">
+      <c r="S3" t="s">
         <v>43</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="T3" t="s">
         <v>44</v>
       </c>
-      <c r="R3" t="s">
+      <c r="U3" t="s">
         <v>54</v>
       </c>
-      <c r="AA3" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="AB3" s="4" t="s">
-        <v>76</v>
+      <c r="AD3" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="AE3" s="4" t="s">
+        <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -862,31 +902,40 @@
         <v>1</v>
       </c>
       <c r="M4">
+        <v>-1</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4">
         <v>0</v>
       </c>
-      <c r="N4" t="s">
+      <c r="P4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q4" t="s">
         <v>7</v>
       </c>
-      <c r="O4" t="s">
+      <c r="R4" t="s">
         <v>13</v>
       </c>
-      <c r="P4" t="s">
+      <c r="S4" t="s">
         <v>43</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="T4" t="s">
         <v>44</v>
       </c>
-      <c r="R4" t="s">
+      <c r="U4" t="s">
         <v>56</v>
       </c>
-      <c r="AA4" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="AB4" s="4" t="s">
-        <v>75</v>
+      <c r="AD4" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="AE4" s="4" t="s">
+        <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -921,31 +970,43 @@
         <v>4</v>
       </c>
       <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>-1</v>
+      </c>
+      <c r="N5">
         <v>0</v>
       </c>
-      <c r="M5">
+      <c r="O5">
         <v>0</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>9</v>
+      </c>
+      <c r="R5" t="s">
         <v>12</v>
       </c>
-      <c r="P5" t="s">
+      <c r="S5" t="s">
         <v>43</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="T5" t="s">
         <v>44</v>
       </c>
-      <c r="R5" t="s">
+      <c r="U5" t="s">
         <v>54</v>
       </c>
-      <c r="AA5" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="AB5" s="4" t="s">
-        <v>74</v>
+      <c r="AD5" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE5" s="4" t="s">
+        <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -983,35 +1044,47 @@
         <v>1</v>
       </c>
       <c r="M6">
+        <v>-1</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
         <v>0</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>9</v>
+      </c>
+      <c r="R6" t="s">
         <v>14</v>
       </c>
-      <c r="P6" t="s">
+      <c r="S6" t="s">
         <v>41</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="T6" t="s">
         <v>42</v>
       </c>
-      <c r="R6" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA6" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="AB6" s="4" t="s">
-        <v>73</v>
+      <c r="U6" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD6" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE6" s="4" t="s">
+        <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="5" t="s">
         <v>49</v>
       </c>
       <c r="D7" t="s">
@@ -1039,44 +1112,56 @@
         <v>5</v>
       </c>
       <c r="L7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M7">
+        <v>-2</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
         <v>0</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>9</v>
+      </c>
+      <c r="R7" t="s">
         <v>13</v>
       </c>
-      <c r="P7" t="s">
+      <c r="S7" t="s">
         <v>45</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="T7" t="s">
         <v>46</v>
       </c>
-      <c r="R7" t="s">
+      <c r="U7" t="s">
         <v>57</v>
       </c>
-      <c r="AA7" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="AB7" s="4" t="s">
-        <v>72</v>
+      <c r="AD7" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AE7" s="4" t="s">
+        <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="5" t="s">
         <v>49</v>
       </c>
       <c r="F8" t="s">
@@ -1085,7 +1170,7 @@
       <c r="G8">
         <v>1</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="5" t="s">
         <v>49</v>
       </c>
       <c r="I8" t="s">
@@ -1098,47 +1183,56 @@
         <v>53</v>
       </c>
       <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="N8">
         <v>2</v>
       </c>
-      <c r="M8">
-        <v>1</v>
-      </c>
-      <c r="N8" t="s">
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="P8" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q8" t="s">
         <v>7</v>
       </c>
-      <c r="O8" t="s">
+      <c r="R8" t="s">
         <v>14</v>
       </c>
-      <c r="P8" t="s">
+      <c r="S8" t="s">
         <v>50</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="T8" t="s">
         <v>51</v>
       </c>
-      <c r="R8" t="s">
+      <c r="U8" t="s">
         <v>58</v>
       </c>
-      <c r="AA8" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="AB8" s="4" t="s">
-        <v>71</v>
+      <c r="AD8" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="AE8" s="4" t="s">
+        <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="5" t="s">
         <v>49</v>
       </c>
       <c r="F9" t="s">
@@ -1147,7 +1241,7 @@
       <c r="G9">
         <v>1</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="5" t="s">
         <v>49</v>
       </c>
       <c r="I9" t="s">
@@ -1160,108 +1254,126 @@
         <v>6</v>
       </c>
       <c r="L9">
-        <v>1</v>
-      </c>
-      <c r="M9">
         <v>0</v>
       </c>
-      <c r="O9" t="s">
+      <c r="M9" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>9</v>
+      </c>
+      <c r="R9" t="s">
         <v>14</v>
       </c>
-      <c r="P9" t="s">
+      <c r="S9" t="s">
         <v>50</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="T9" t="s">
         <v>51</v>
       </c>
-      <c r="R9" t="s">
+      <c r="U9" t="s">
         <v>55</v>
       </c>
-      <c r="AA9" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="AB9" s="4" t="s">
-        <v>69</v>
+      <c r="AD9" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE9" s="4" t="s">
+        <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="G12" t="s">
-        <v>85</v>
-      </c>
-      <c r="L12">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12" t="s">
+        <v>88</v>
+      </c>
+      <c r="N12">
         <v>-1</v>
       </c>
-      <c r="M12" t="s">
+      <c r="O12" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="G13" t="s">
-        <v>86</v>
-      </c>
-      <c r="L13">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13" t="s">
+        <v>89</v>
+      </c>
+      <c r="N13">
         <v>0</v>
       </c>
-      <c r="M13" t="s">
-        <v>65</v>
+      <c r="O13" t="s">
+        <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="L14">
-        <v>1</v>
-      </c>
-      <c r="M14" t="s">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="N14">
+        <v>1</v>
+      </c>
+      <c r="O14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="N15">
+        <v>2</v>
+      </c>
+      <c r="O15" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="L15">
-        <v>2</v>
-      </c>
-      <c r="M15" t="s">
-        <v>68</v>
+    <row r="18" spans="15:16" x14ac:dyDescent="0.25">
+      <c r="O18">
+        <v>-1</v>
+      </c>
+      <c r="P18" t="s">
+        <v>61</v>
       </c>
     </row>
-    <row r="18" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M18">
-        <v>-1</v>
-      </c>
-      <c r="N18" t="s">
-        <v>61</v>
+    <row r="19" spans="15:16" x14ac:dyDescent="0.25">
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19" t="s">
+        <v>59</v>
       </c>
     </row>
-    <row r="19" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M19">
-        <v>0</v>
-      </c>
-      <c r="N19" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M20">
-        <v>1</v>
-      </c>
-      <c r="N20" t="s">
+    <row r="20" spans="15:16" x14ac:dyDescent="0.25">
+      <c r="O20">
+        <v>1</v>
+      </c>
+      <c r="P20" t="s">
         <v>60</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="AA3" r:id="rId1" location="transformers.BertTokenizer" xr:uid="{34D2F53E-DD38-4D02-B9D7-EEB3C73565A4}"/>
-    <hyperlink ref="AA4" r:id="rId2" location="transformers.AlbertTokenizer" xr:uid="{1C747986-9A2C-4D37-85D4-551E037E79AF}"/>
-    <hyperlink ref="AA5" r:id="rId3" location="transformers.DistilBertTokenizer" xr:uid="{4557F4E1-3CF5-452D-B493-FBA68FEF70C1}"/>
-    <hyperlink ref="AA6" r:id="rId4" location="transformers.RobertaTokenizer" xr:uid="{38642F05-9C73-4563-BF96-AEE8C072DC8E}"/>
-    <hyperlink ref="AA7" r:id="rId5" location="transformers.XLNetTokenizer" xr:uid="{287DC99E-D4A0-4091-81B9-FD3CC7A6D5AB}"/>
-    <hyperlink ref="AA8" r:id="rId6" location="transformers.OpenAIGPTTokenizer" xr:uid="{1381AF7A-FED8-43A8-B952-743B3E821ABF}"/>
-    <hyperlink ref="AA9" r:id="rId7" location="transformers.GPT2Tokenizer" xr:uid="{D91A5263-1AFB-40F8-BF67-C0F7CF6DD3B8}"/>
-    <hyperlink ref="AB3" r:id="rId8" xr:uid="{5ED3647C-C8FA-443D-AAEB-9454BBCF6176}"/>
-    <hyperlink ref="AB4" r:id="rId9" xr:uid="{118612AF-F178-449D-94F5-EA8FCCE6B629}"/>
-    <hyperlink ref="AB5" r:id="rId10" xr:uid="{9F819B38-1C37-4436-86A4-26447E432B97}"/>
-    <hyperlink ref="AB6" r:id="rId11" xr:uid="{3E18BD0A-C819-47DD-AF95-3DFEF2DEB3D5}"/>
-    <hyperlink ref="AB7" r:id="rId12" xr:uid="{E2C80B92-5270-44E6-BA42-98A672C126C8}"/>
-    <hyperlink ref="AB8" r:id="rId13" xr:uid="{65DBFE01-0236-40D1-BAA2-DBC7A7D06BBE}"/>
-    <hyperlink ref="AB9" r:id="rId14" xr:uid="{31303705-0E07-4F0C-A889-CB48F2A8D49E}"/>
+    <hyperlink ref="AD3" r:id="rId1" location="transformers.BertTokenizer" xr:uid="{34D2F53E-DD38-4D02-B9D7-EEB3C73565A4}"/>
+    <hyperlink ref="AD4" r:id="rId2" location="transformers.AlbertTokenizer" xr:uid="{1C747986-9A2C-4D37-85D4-551E037E79AF}"/>
+    <hyperlink ref="AD5" r:id="rId3" location="transformers.DistilBertTokenizer" xr:uid="{4557F4E1-3CF5-452D-B493-FBA68FEF70C1}"/>
+    <hyperlink ref="AD6" r:id="rId4" location="transformers.RobertaTokenizer" xr:uid="{38642F05-9C73-4563-BF96-AEE8C072DC8E}"/>
+    <hyperlink ref="AD7" r:id="rId5" location="transformers.XLNetTokenizer" xr:uid="{287DC99E-D4A0-4091-81B9-FD3CC7A6D5AB}"/>
+    <hyperlink ref="AD8" r:id="rId6" location="transformers.OpenAIGPTTokenizer" xr:uid="{1381AF7A-FED8-43A8-B952-743B3E821ABF}"/>
+    <hyperlink ref="AD9" r:id="rId7" location="transformers.GPT2Tokenizer" xr:uid="{D91A5263-1AFB-40F8-BF67-C0F7CF6DD3B8}"/>
+    <hyperlink ref="AE3" r:id="rId8" xr:uid="{5ED3647C-C8FA-443D-AAEB-9454BBCF6176}"/>
+    <hyperlink ref="AE4" r:id="rId9" xr:uid="{118612AF-F178-449D-94F5-EA8FCCE6B629}"/>
+    <hyperlink ref="AE5" r:id="rId10" xr:uid="{9F819B38-1C37-4436-86A4-26447E432B97}"/>
+    <hyperlink ref="AE6" r:id="rId11" xr:uid="{3E18BD0A-C819-47DD-AF95-3DFEF2DEB3D5}"/>
+    <hyperlink ref="AE7" r:id="rId12" xr:uid="{E2C80B92-5270-44E6-BA42-98A672C126C8}"/>
+    <hyperlink ref="AE8" r:id="rId13" xr:uid="{65DBFE01-0236-40D1-BAA2-DBC7A7D06BBE}"/>
+    <hyperlink ref="AE9" r:id="rId14" xr:uid="{31303705-0E07-4F0C-A889-CB48F2A8D49E}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId15"/>

</xml_diff>

<commit_message>
Classe e testes XMLRoberta
</commit_message>
<xml_diff>
--- a/modelos.xlsx
+++ b/modelos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\osmar\Documentos\GitHub\texto-transformer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{968172B3-96E2-4178-A4D1-9D3F137C9D75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DDAD328-3C44-4608-87AA-F22B9E16A59E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{ADA84CBB-E06D-42EE-8062-4654A38564A2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="96">
   <si>
     <t>modelo</t>
   </si>
@@ -164,9 +164,6 @@
     <t>&lt;s&gt; X &lt;/s&gt;</t>
   </si>
   <si>
-    <t>&lt;s&gt; A &lt;/s&gt;&lt;/s&gt; B &lt;/s&gt;</t>
-  </si>
-  <si>
     <t>[CLS] X [SEP]</t>
   </si>
   <si>
@@ -306,6 +303,27 @@
   </si>
   <si>
     <t>preenchimento pad a direita</t>
+  </si>
+  <si>
+    <t>XLMRoberta</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/docs/transformers/model_doc/xlm-roberta#transformers.XLMRobertaTokenizer</t>
+  </si>
+  <si>
+    <t>https://github.com/huggingface/transformers/blob/v4.30.0/src/transformers/models/xlm_roberta/tokenization_xlm_roberta.py</t>
+  </si>
+  <si>
+    <t>&lt;s&gt; A &lt;/s&gt;&lt;s&gt; B &lt;/s&gt;</t>
+  </si>
+  <si>
+    <t>Posição do primeiro token válido</t>
+  </si>
+  <si>
+    <t>Posição do último token válido</t>
+  </si>
+  <si>
+    <t>['&lt;s&gt;', '▁Fresh', '▁sea', '▁bas', 's', '▁is', '▁a', '▁great', '▁de', 'lica', 'cy', '.', '&lt;/s&gt;']</t>
   </si>
 </sst>
 </file>
@@ -697,10 +715,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D3D3DC9-8A8A-4ECE-AF2B-5AE8D9558D5B}">
-  <dimension ref="A2:AE20"/>
+  <dimension ref="A2:AE22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -742,7 +760,7 @@
         <v>22</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>25</v>
@@ -754,22 +772,22 @@
         <v>16</v>
       </c>
       <c r="K2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="N2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>85</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>10</v>
@@ -787,15 +805,15 @@
         <v>3</v>
       </c>
       <c r="AD2" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AE2" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>31</v>
@@ -810,22 +828,22 @@
         <v>31</v>
       </c>
       <c r="F3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="3">
+        <v>24</v>
+      </c>
+      <c r="G3">
         <v>1</v>
       </c>
       <c r="H3" t="s">
         <v>26</v>
       </c>
       <c r="I3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J3" t="s">
         <v>7</v>
       </c>
       <c r="K3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L3">
         <v>1</v>
@@ -834,7 +852,7 @@
         <v>-1</v>
       </c>
       <c r="N3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O3">
         <v>0</v>
@@ -843,30 +861,30 @@
         <v>9</v>
       </c>
       <c r="Q3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="R3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="S3" t="s">
+        <v>42</v>
+      </c>
+      <c r="T3" t="s">
         <v>43</v>
       </c>
-      <c r="T3" t="s">
-        <v>44</v>
-      </c>
       <c r="U3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AD3" s="4" t="s">
         <v>77</v>
       </c>
       <c r="AE3" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
         <v>31</v>
@@ -881,22 +899,22 @@
         <v>31</v>
       </c>
       <c r="F4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4">
+        <v>23</v>
+      </c>
+      <c r="G4" s="3">
         <v>1</v>
       </c>
       <c r="H4" t="s">
         <v>26</v>
       </c>
       <c r="I4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J4" t="s">
         <v>7</v>
       </c>
       <c r="K4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L4">
         <v>1</v>
@@ -905,7 +923,7 @@
         <v>-1</v>
       </c>
       <c r="N4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O4">
         <v>0</v>
@@ -914,22 +932,22 @@
         <v>9</v>
       </c>
       <c r="Q4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="R4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="S4" t="s">
+        <v>42</v>
+      </c>
+      <c r="T4" t="s">
         <v>43</v>
       </c>
-      <c r="T4" t="s">
-        <v>44</v>
-      </c>
       <c r="U4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="AD4" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="AE4" s="4" t="s">
         <v>74</v>
@@ -991,48 +1009,48 @@
         <v>12</v>
       </c>
       <c r="S5" t="s">
+        <v>42</v>
+      </c>
+      <c r="T5" t="s">
         <v>43</v>
       </c>
-      <c r="T5" t="s">
-        <v>44</v>
-      </c>
       <c r="U5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AD5" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AE5" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6" t="s">
-        <v>33</v>
+        <v>47</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="F6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G6">
         <v>1</v>
       </c>
-      <c r="H6" t="s">
-        <v>27</v>
+      <c r="H6" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="I6" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="J6" t="s">
         <v>7</v>
@@ -1041,10 +1059,10 @@
         <v>6</v>
       </c>
       <c r="L6">
-        <v>1</v>
-      </c>
-      <c r="M6">
-        <v>-1</v>
+        <v>0</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="N6">
         <v>1</v>
@@ -1062,60 +1080,60 @@
         <v>14</v>
       </c>
       <c r="S6" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="T6" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="U6" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="AD6" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AE6" s="4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>49</v>
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" t="s">
+        <v>35</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F7" t="s">
         <v>24</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" t="s">
         <v>27</v>
       </c>
       <c r="I7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J7" t="s">
         <v>7</v>
       </c>
       <c r="K7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M7">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="N7">
         <v>1</v>
@@ -1124,25 +1142,25 @@
         <v>0</v>
       </c>
       <c r="P7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="Q7" t="s">
         <v>9</v>
       </c>
       <c r="R7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="S7" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="T7" t="s">
-        <v>46</v>
+        <v>92</v>
       </c>
       <c r="U7" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="AD7" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="AE7" s="4" t="s">
         <v>71</v>
@@ -1150,19 +1168,19 @@
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F8" t="s">
         <v>23</v>
@@ -1171,7 +1189,7 @@
         <v>1</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I8" t="s">
         <v>18</v>
@@ -1180,13 +1198,13 @@
         <v>7</v>
       </c>
       <c r="K8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L8">
         <v>0</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N8">
         <v>2</v>
@@ -1204,60 +1222,60 @@
         <v>14</v>
       </c>
       <c r="S8" t="s">
+        <v>49</v>
+      </c>
+      <c r="T8" t="s">
         <v>50</v>
       </c>
-      <c r="T8" t="s">
-        <v>51</v>
-      </c>
       <c r="U8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AD8" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AE8" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>49</v>
+        <v>89</v>
+      </c>
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" t="s">
+        <v>33</v>
       </c>
       <c r="F9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G9">
         <v>1</v>
       </c>
-      <c r="H9" s="5" t="s">
-        <v>49</v>
+      <c r="H9" t="s">
+        <v>27</v>
       </c>
       <c r="I9" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="J9" t="s">
         <v>7</v>
       </c>
       <c r="K9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L9">
-        <v>0</v>
-      </c>
-      <c r="M9" s="5" t="s">
-        <v>49</v>
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <v>-1</v>
       </c>
       <c r="N9">
         <v>1</v>
@@ -1266,64 +1284,135 @@
         <v>0</v>
       </c>
       <c r="P9" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="Q9" t="s">
         <v>9</v>
       </c>
       <c r="R9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="S9" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="T9" t="s">
-        <v>51</v>
+        <v>92</v>
       </c>
       <c r="U9" t="s">
-        <v>55</v>
+        <v>95</v>
       </c>
       <c r="AD9" s="4" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="AE9" s="4" t="s">
-        <v>68</v>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10" t="s">
+        <v>27</v>
+      </c>
+      <c r="I10" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" t="s">
+        <v>7</v>
+      </c>
+      <c r="K10" t="s">
+        <v>5</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>-2</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>9</v>
+      </c>
+      <c r="R10" t="s">
+        <v>13</v>
+      </c>
+      <c r="S10" t="s">
+        <v>44</v>
+      </c>
+      <c r="T10" t="s">
+        <v>45</v>
+      </c>
+      <c r="U10" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD10" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE10" s="4" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12" t="s">
-        <v>88</v>
-      </c>
       <c r="N12">
         <v>-1</v>
       </c>
       <c r="O12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="G13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="N13">
         <v>0</v>
       </c>
       <c r="O13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14" t="s">
+        <v>88</v>
+      </c>
       <c r="N14">
         <v>1</v>
       </c>
       <c r="O14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
@@ -1331,49 +1420,59 @@
         <v>2</v>
       </c>
       <c r="O15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
-    <row r="18" spans="15:16" x14ac:dyDescent="0.25">
-      <c r="O18">
+    <row r="17" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L17" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M18" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="O20">
         <v>-1</v>
-      </c>
-      <c r="P18" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="19" spans="15:16" x14ac:dyDescent="0.25">
-      <c r="O19">
-        <v>0</v>
-      </c>
-      <c r="P19" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="15:16" x14ac:dyDescent="0.25">
-      <c r="O20">
-        <v>1</v>
       </c>
       <c r="P20" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="O22">
+        <v>1</v>
+      </c>
+      <c r="P22" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="AD3" r:id="rId1" location="transformers.BertTokenizer" xr:uid="{34D2F53E-DD38-4D02-B9D7-EEB3C73565A4}"/>
-    <hyperlink ref="AD4" r:id="rId2" location="transformers.AlbertTokenizer" xr:uid="{1C747986-9A2C-4D37-85D4-551E037E79AF}"/>
+    <hyperlink ref="AD4" r:id="rId1" location="transformers.BertTokenizer" xr:uid="{34D2F53E-DD38-4D02-B9D7-EEB3C73565A4}"/>
+    <hyperlink ref="AD3" r:id="rId2" location="transformers.AlbertTokenizer" xr:uid="{1C747986-9A2C-4D37-85D4-551E037E79AF}"/>
     <hyperlink ref="AD5" r:id="rId3" location="transformers.DistilBertTokenizer" xr:uid="{4557F4E1-3CF5-452D-B493-FBA68FEF70C1}"/>
-    <hyperlink ref="AD6" r:id="rId4" location="transformers.RobertaTokenizer" xr:uid="{38642F05-9C73-4563-BF96-AEE8C072DC8E}"/>
-    <hyperlink ref="AD7" r:id="rId5" location="transformers.XLNetTokenizer" xr:uid="{287DC99E-D4A0-4091-81B9-FD3CC7A6D5AB}"/>
+    <hyperlink ref="AD7" r:id="rId4" location="transformers.RobertaTokenizer" xr:uid="{38642F05-9C73-4563-BF96-AEE8C072DC8E}"/>
+    <hyperlink ref="AD10" r:id="rId5" location="transformers.XLNetTokenizer" xr:uid="{287DC99E-D4A0-4091-81B9-FD3CC7A6D5AB}"/>
     <hyperlink ref="AD8" r:id="rId6" location="transformers.OpenAIGPTTokenizer" xr:uid="{1381AF7A-FED8-43A8-B952-743B3E821ABF}"/>
-    <hyperlink ref="AD9" r:id="rId7" location="transformers.GPT2Tokenizer" xr:uid="{D91A5263-1AFB-40F8-BF67-C0F7CF6DD3B8}"/>
-    <hyperlink ref="AE3" r:id="rId8" xr:uid="{5ED3647C-C8FA-443D-AAEB-9454BBCF6176}"/>
-    <hyperlink ref="AE4" r:id="rId9" xr:uid="{118612AF-F178-449D-94F5-EA8FCCE6B629}"/>
+    <hyperlink ref="AD6" r:id="rId7" location="transformers.GPT2Tokenizer" xr:uid="{D91A5263-1AFB-40F8-BF67-C0F7CF6DD3B8}"/>
+    <hyperlink ref="AE4" r:id="rId8" xr:uid="{5ED3647C-C8FA-443D-AAEB-9454BBCF6176}"/>
+    <hyperlink ref="AE3" r:id="rId9" xr:uid="{118612AF-F178-449D-94F5-EA8FCCE6B629}"/>
     <hyperlink ref="AE5" r:id="rId10" xr:uid="{9F819B38-1C37-4436-86A4-26447E432B97}"/>
-    <hyperlink ref="AE6" r:id="rId11" xr:uid="{3E18BD0A-C819-47DD-AF95-3DFEF2DEB3D5}"/>
-    <hyperlink ref="AE7" r:id="rId12" xr:uid="{E2C80B92-5270-44E6-BA42-98A672C126C8}"/>
+    <hyperlink ref="AE7" r:id="rId11" xr:uid="{3E18BD0A-C819-47DD-AF95-3DFEF2DEB3D5}"/>
+    <hyperlink ref="AE10" r:id="rId12" xr:uid="{E2C80B92-5270-44E6-BA42-98A672C126C8}"/>
     <hyperlink ref="AE8" r:id="rId13" xr:uid="{65DBFE01-0236-40D1-BAA2-DBC7A7D06BBE}"/>
-    <hyperlink ref="AE9" r:id="rId14" xr:uid="{31303705-0E07-4F0C-A889-CB48F2A8D49E}"/>
+    <hyperlink ref="AE6" r:id="rId14" xr:uid="{31303705-0E07-4F0C-A889-CB48F2A8D49E}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId15"/>
@@ -1381,6 +1480,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100886399F21440F54B81A4893F74DA4F94" ma:contentTypeVersion="8" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="91b6ab92f34ab688a19900d483ae7505">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0190bee1-42b9-4362-9dc8-2229f310bd34" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d4f82e64d1772ab8a19658e1978de7e8" ns3:_="">
     <xsd:import namespace="0190bee1-42b9-4362-9dc8-2229f310bd34"/>
@@ -1550,15 +1658,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1566,6 +1665,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6C04E1C-86C9-4DFF-AFD3-8243B20410CC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FBDDB8E-E50B-4DEA-B8C8-CD7F650AB124}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1579,14 +1686,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6C04E1C-86C9-4DFF-AFD3-8243B20410CC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Ajuste na ordem das constantes.
</commit_message>
<xml_diff>
--- a/modelos.xlsx
+++ b/modelos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\osmar\Documentos\GitHub\texto-transformer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D4EAA60-10DC-49C4-8873-46447B92A46D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E28F0E42-1902-4C86-89EC-9955FC61A812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{ADA84CBB-E06D-42EE-8062-4654A38564A2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="105">
   <si>
     <t>modelo</t>
   </si>
@@ -86,9 +86,6 @@
     <t>Wordpiece</t>
   </si>
   <si>
-    <t>subtoken</t>
-  </si>
-  <si>
     <t>Â</t>
   </si>
   <si>
@@ -218,12 +215,6 @@
     <t>sem subtoken</t>
   </si>
   <si>
-    <t>separador_subtoken</t>
-  </si>
-  <si>
-    <t>separador_subtoken_position</t>
-  </si>
-  <si>
     <t>nos subtokens(menos primeiro)</t>
   </si>
   <si>
@@ -284,18 +275,6 @@
     <t>https://huggingface.co/docs/transformers/model_doc/openai-gpt#transformers.OpenAIGPTTokenizer</t>
   </si>
   <si>
-    <t>separador_subtoken_repeticao</t>
-  </si>
-  <si>
-    <t>primeiro_token_sem_separador</t>
-  </si>
-  <si>
-    <t>posicao_token_final</t>
-  </si>
-  <si>
-    <t>posicao_token_inicio</t>
-  </si>
-  <si>
     <t>preenchimento pad a esquerda</t>
   </si>
   <si>
@@ -324,6 +303,54 @@
   </si>
   <si>
     <t>GPT2</t>
+  </si>
+  <si>
+    <t>TOKEN_INICIO</t>
+  </si>
+  <si>
+    <t>SEPARADOR_SUBTOKEN</t>
+  </si>
+  <si>
+    <t>SERAPADOR_SUBTOKEN_REPETICAO</t>
+  </si>
+  <si>
+    <t>SEPARADOR_SUBTOKEN_POSICAO</t>
+  </si>
+  <si>
+    <t>PRIMEIRO_TOKEN_SEM_SEPARADOR</t>
+  </si>
+  <si>
+    <t>DO_LOWER_CASE</t>
+  </si>
+  <si>
+    <t>POSICAO_TOKEN_INICIO</t>
+  </si>
+  <si>
+    <t>TOKEN_FIM</t>
+  </si>
+  <si>
+    <t>POSICAO_TOKEN_FINAL</t>
+  </si>
+  <si>
+    <t>TOKEN_SEPARADOR</t>
+  </si>
+  <si>
+    <t>TOKEN_CLASSIFICACAO</t>
+  </si>
+  <si>
+    <t>TOKEN_PADDING</t>
+  </si>
+  <si>
+    <t>PADDING_SIDE</t>
+  </si>
+  <si>
+    <t>TOKEN_MASCARA</t>
+  </si>
+  <si>
+    <t>TOKEN_DESCONHECIDO</t>
+  </si>
+  <si>
+    <t>Nomes huggingface</t>
   </si>
 </sst>
 </file>
@@ -715,10 +742,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D3D3DC9-8A8A-4ECE-AF2B-5AE8D9558D5B}">
-  <dimension ref="A2:AD22"/>
+  <dimension ref="A2:AC23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Z15" sqref="Z15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -732,455 +759,412 @@
     <col min="7" max="7" width="6.140625" customWidth="1"/>
     <col min="8" max="8" width="8" customWidth="1"/>
     <col min="9" max="9" width="7.5703125" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" customWidth="1"/>
-    <col min="11" max="16" width="5.5703125" customWidth="1"/>
-    <col min="17" max="17" width="6.140625" customWidth="1"/>
-    <col min="19" max="19" width="13" customWidth="1"/>
-    <col min="20" max="20" width="20" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="15" width="5.5703125" customWidth="1"/>
+    <col min="16" max="16" width="6.140625" customWidth="1"/>
+    <col min="18" max="18" width="13" customWidth="1"/>
+    <col min="19" max="19" width="20" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="AB2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="B3" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB3" s="1"/>
+      <c r="AC3" s="1"/>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="AC2" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AD2" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" t="s">
-        <v>7</v>
-      </c>
-      <c r="K3" t="s">
-        <v>5</v>
-      </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
-      <c r="M3">
-        <v>-1</v>
-      </c>
-      <c r="N3">
-        <v>1</v>
-      </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
-      <c r="P3" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>7</v>
-      </c>
-      <c r="R3" t="s">
-        <v>13</v>
-      </c>
-      <c r="S3" t="s">
-        <v>42</v>
-      </c>
-      <c r="T3" t="s">
-        <v>43</v>
-      </c>
-      <c r="U3" t="s">
-        <v>54</v>
-      </c>
-      <c r="AC3" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="AD3" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>31</v>
-      </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F4" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4">
         <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J4" t="s">
-        <v>7</v>
-      </c>
-      <c r="K4" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
       </c>
       <c r="L4">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="M4">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="N4">
         <v>0</v>
       </c>
-      <c r="O4">
-        <v>0</v>
+      <c r="O4" t="s">
+        <v>9</v>
       </c>
       <c r="P4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="Q4" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="R4" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="S4" t="s">
         <v>42</v>
       </c>
       <c r="T4" t="s">
-        <v>43</v>
-      </c>
-      <c r="U4" t="s">
-        <v>52</v>
+        <v>53</v>
+      </c>
+      <c r="AB4" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="AC4" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="AD4" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5">
+        <v>22</v>
+      </c>
+      <c r="G5" s="3">
         <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J5" t="s">
-        <v>9</v>
-      </c>
-      <c r="K5" t="s">
         <v>4</v>
       </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
       <c r="L5">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="M5">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="N5">
         <v>0</v>
       </c>
-      <c r="O5">
-        <v>0</v>
+      <c r="O5" t="s">
+        <v>9</v>
       </c>
       <c r="P5" t="s">
         <v>9</v>
       </c>
       <c r="Q5" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="R5" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="S5" t="s">
         <v>42</v>
       </c>
       <c r="T5" t="s">
-        <v>43</v>
-      </c>
-      <c r="U5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB5" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="AC5" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>-1</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6" t="s">
+        <v>9</v>
+      </c>
+      <c r="P6" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>12</v>
+      </c>
+      <c r="R6" t="s">
+        <v>41</v>
+      </c>
+      <c r="S6" t="s">
+        <v>42</v>
+      </c>
+      <c r="T6" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB6" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="AC6" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="I7" t="s">
+        <v>46</v>
+      </c>
+      <c r="J7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7" t="s">
+        <v>7</v>
+      </c>
+      <c r="P7" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>14</v>
+      </c>
+      <c r="R7" t="s">
+        <v>47</v>
+      </c>
+      <c r="S7" t="s">
+        <v>48</v>
+      </c>
+      <c r="T7" t="s">
         <v>52</v>
       </c>
-      <c r="AC5" s="4" t="s">
+      <c r="AB7" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="AD5" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="I6" t="s">
-        <v>47</v>
-      </c>
-      <c r="J6" t="s">
-        <v>7</v>
-      </c>
-      <c r="K6" t="s">
-        <v>6</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-      <c r="M6" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="N6">
-        <v>1</v>
-      </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
-      <c r="P6" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>9</v>
-      </c>
-      <c r="R6" t="s">
-        <v>14</v>
-      </c>
-      <c r="S6" t="s">
-        <v>48</v>
-      </c>
-      <c r="T6" t="s">
-        <v>49</v>
-      </c>
-      <c r="U6" t="s">
-        <v>53</v>
-      </c>
-      <c r="AC6" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="AD6" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7" t="s">
-        <v>27</v>
-      </c>
-      <c r="I7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J7" t="s">
-        <v>7</v>
-      </c>
-      <c r="K7" t="s">
-        <v>6</v>
-      </c>
-      <c r="L7">
-        <v>1</v>
-      </c>
-      <c r="M7">
-        <v>-1</v>
-      </c>
-      <c r="N7">
-        <v>1</v>
-      </c>
-      <c r="O7">
-        <v>0</v>
-      </c>
-      <c r="P7" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>9</v>
-      </c>
-      <c r="R7" t="s">
-        <v>14</v>
-      </c>
-      <c r="S7" t="s">
-        <v>41</v>
-      </c>
-      <c r="T7" t="s">
-        <v>91</v>
-      </c>
-      <c r="U7" t="s">
+      <c r="AC7" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="AC7" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="AD7" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>47</v>
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" t="s">
+        <v>32</v>
       </c>
       <c r="F8" t="s">
         <v>23</v>
@@ -1188,291 +1172,350 @@
       <c r="G8">
         <v>1</v>
       </c>
-      <c r="H8" s="5" t="s">
-        <v>47</v>
+      <c r="H8" t="s">
+        <v>26</v>
       </c>
       <c r="I8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J8" t="s">
+        <v>6</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>-1</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8" t="s">
         <v>7</v>
-      </c>
-      <c r="K8" t="s">
-        <v>51</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-      <c r="M8" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="N8">
-        <v>2</v>
-      </c>
-      <c r="O8">
-        <v>1</v>
       </c>
       <c r="P8" t="s">
         <v>9</v>
       </c>
       <c r="Q8" t="s">
+        <v>14</v>
+      </c>
+      <c r="R8" t="s">
+        <v>40</v>
+      </c>
+      <c r="S8" t="s">
+        <v>84</v>
+      </c>
+      <c r="T8" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB8" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC8" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="I9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" t="s">
+        <v>50</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="M9">
+        <v>2</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9" t="s">
+        <v>9</v>
+      </c>
+      <c r="P9" t="s">
         <v>7</v>
       </c>
-      <c r="R8" t="s">
+      <c r="Q9" t="s">
         <v>14</v>
       </c>
-      <c r="S8" t="s">
+      <c r="R9" t="s">
+        <v>47</v>
+      </c>
+      <c r="S9" t="s">
         <v>48</v>
       </c>
-      <c r="T8" t="s">
-        <v>49</v>
-      </c>
-      <c r="U8" t="s">
-        <v>56</v>
-      </c>
-      <c r="AC8" s="4" t="s">
+      <c r="T9" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB9" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC9" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="AD8" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" t="s">
-        <v>35</v>
-      </c>
-      <c r="E9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9" t="s">
-        <v>24</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-      <c r="H9" t="s">
-        <v>27</v>
-      </c>
-      <c r="I9" t="s">
-        <v>18</v>
-      </c>
-      <c r="J9" t="s">
-        <v>7</v>
-      </c>
-      <c r="K9" t="s">
-        <v>5</v>
-      </c>
-      <c r="L9">
-        <v>1</v>
-      </c>
-      <c r="M9">
-        <v>-1</v>
-      </c>
-      <c r="N9">
-        <v>1</v>
-      </c>
-      <c r="O9">
-        <v>0</v>
-      </c>
-      <c r="P9" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>9</v>
-      </c>
-      <c r="R9" t="s">
-        <v>13</v>
-      </c>
-      <c r="S9" t="s">
-        <v>41</v>
-      </c>
-      <c r="T9" t="s">
-        <v>91</v>
-      </c>
-      <c r="U9" t="s">
-        <v>94</v>
-      </c>
-      <c r="AC9" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="AD9" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>47</v>
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E10" t="s">
         <v>32</v>
       </c>
       <c r="F10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10" t="s">
+        <v>26</v>
+      </c>
+      <c r="I10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" t="s">
+        <v>5</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>-1</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+      <c r="N10">
         <v>0</v>
       </c>
-      <c r="H10" t="s">
-        <v>27</v>
-      </c>
-      <c r="I10" t="s">
-        <v>18</v>
-      </c>
-      <c r="J10" t="s">
-        <v>7</v>
-      </c>
-      <c r="K10" t="s">
-        <v>5</v>
-      </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
-      <c r="M10">
-        <v>-2</v>
-      </c>
-      <c r="N10">
-        <v>1</v>
-      </c>
-      <c r="O10">
-        <v>0</v>
+      <c r="O10" t="s">
+        <v>9</v>
       </c>
       <c r="P10" t="s">
         <v>9</v>
       </c>
       <c r="Q10" t="s">
+        <v>13</v>
+      </c>
+      <c r="R10" t="s">
+        <v>40</v>
+      </c>
+      <c r="S10" t="s">
+        <v>84</v>
+      </c>
+      <c r="T10" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB10" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC10" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11" t="s">
+        <v>26</v>
+      </c>
+      <c r="I11" t="s">
+        <v>17</v>
+      </c>
+      <c r="J11" t="s">
+        <v>5</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>-2</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11" t="s">
         <v>9</v>
       </c>
-      <c r="R10" t="s">
+      <c r="P11" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q11" t="s">
         <v>13</v>
       </c>
-      <c r="S10" t="s">
+      <c r="R11" t="s">
+        <v>43</v>
+      </c>
+      <c r="S11" t="s">
         <v>44</v>
       </c>
-      <c r="T10" t="s">
-        <v>45</v>
-      </c>
-      <c r="U10" t="s">
-        <v>55</v>
-      </c>
-      <c r="AC10" s="4" t="s">
+      <c r="T11" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB11" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC11" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="M13">
+        <v>-1</v>
+      </c>
+      <c r="N13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14" t="s">
         <v>79</v>
       </c>
-      <c r="AD10" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="N12">
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15" t="s">
+        <v>80</v>
+      </c>
+      <c r="M15">
+        <v>1</v>
+      </c>
+      <c r="N15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="M16">
+        <v>2</v>
+      </c>
+      <c r="N16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K18" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="L19" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="N21">
         <v>-1</v>
       </c>
-      <c r="O12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="G13">
+      <c r="O21" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="N22">
         <v>0</v>
       </c>
-      <c r="H13" t="s">
-        <v>86</v>
-      </c>
-      <c r="N13">
-        <v>0</v>
-      </c>
-      <c r="O13" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="G14">
-        <v>1</v>
-      </c>
-      <c r="H14" t="s">
-        <v>87</v>
-      </c>
-      <c r="N14">
-        <v>1</v>
-      </c>
-      <c r="O14" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="N15">
-        <v>2</v>
-      </c>
-      <c r="O15" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="17" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="L17" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="18" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="M18" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="20" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="O20">
-        <v>-1</v>
-      </c>
-      <c r="P20" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="21" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="O21">
-        <v>0</v>
-      </c>
-      <c r="P21" t="s">
+      <c r="O22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="N23">
+        <v>1</v>
+      </c>
+      <c r="O23" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="22" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="O22">
-        <v>1</v>
-      </c>
-      <c r="P22" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="AC4" r:id="rId1" location="transformers.BertTokenizer" xr:uid="{34D2F53E-DD38-4D02-B9D7-EEB3C73565A4}"/>
-    <hyperlink ref="AC3" r:id="rId2" location="transformers.AlbertTokenizer" xr:uid="{1C747986-9A2C-4D37-85D4-551E037E79AF}"/>
-    <hyperlink ref="AC5" r:id="rId3" location="transformers.DistilBertTokenizer" xr:uid="{4557F4E1-3CF5-452D-B493-FBA68FEF70C1}"/>
-    <hyperlink ref="AC7" r:id="rId4" location="transformers.RobertaTokenizer" xr:uid="{38642F05-9C73-4563-BF96-AEE8C072DC8E}"/>
-    <hyperlink ref="AC10" r:id="rId5" location="transformers.XLNetTokenizer" xr:uid="{287DC99E-D4A0-4091-81B9-FD3CC7A6D5AB}"/>
-    <hyperlink ref="AC8" r:id="rId6" location="transformers.OpenAIGPTTokenizer" xr:uid="{1381AF7A-FED8-43A8-B952-743B3E821ABF}"/>
-    <hyperlink ref="AC6" r:id="rId7" location="transformers.GPT2Tokenizer" xr:uid="{D91A5263-1AFB-40F8-BF67-C0F7CF6DD3B8}"/>
-    <hyperlink ref="AD4" r:id="rId8" xr:uid="{5ED3647C-C8FA-443D-AAEB-9454BBCF6176}"/>
-    <hyperlink ref="AD3" r:id="rId9" xr:uid="{118612AF-F178-449D-94F5-EA8FCCE6B629}"/>
-    <hyperlink ref="AD5" r:id="rId10" xr:uid="{9F819B38-1C37-4436-86A4-26447E432B97}"/>
-    <hyperlink ref="AD7" r:id="rId11" xr:uid="{3E18BD0A-C819-47DD-AF95-3DFEF2DEB3D5}"/>
-    <hyperlink ref="AD10" r:id="rId12" xr:uid="{E2C80B92-5270-44E6-BA42-98A672C126C8}"/>
-    <hyperlink ref="AD8" r:id="rId13" xr:uid="{65DBFE01-0236-40D1-BAA2-DBC7A7D06BBE}"/>
-    <hyperlink ref="AD6" r:id="rId14" xr:uid="{31303705-0E07-4F0C-A889-CB48F2A8D49E}"/>
+    <hyperlink ref="AB5" r:id="rId1" location="transformers.BertTokenizer" xr:uid="{34D2F53E-DD38-4D02-B9D7-EEB3C73565A4}"/>
+    <hyperlink ref="AB4" r:id="rId2" location="transformers.AlbertTokenizer" xr:uid="{1C747986-9A2C-4D37-85D4-551E037E79AF}"/>
+    <hyperlink ref="AB6" r:id="rId3" location="transformers.DistilBertTokenizer" xr:uid="{4557F4E1-3CF5-452D-B493-FBA68FEF70C1}"/>
+    <hyperlink ref="AB8" r:id="rId4" location="transformers.RobertaTokenizer" xr:uid="{38642F05-9C73-4563-BF96-AEE8C072DC8E}"/>
+    <hyperlink ref="AB11" r:id="rId5" location="transformers.XLNetTokenizer" xr:uid="{287DC99E-D4A0-4091-81B9-FD3CC7A6D5AB}"/>
+    <hyperlink ref="AB9" r:id="rId6" location="transformers.OpenAIGPTTokenizer" xr:uid="{1381AF7A-FED8-43A8-B952-743B3E821ABF}"/>
+    <hyperlink ref="AB7" r:id="rId7" location="transformers.GPT2Tokenizer" xr:uid="{D91A5263-1AFB-40F8-BF67-C0F7CF6DD3B8}"/>
+    <hyperlink ref="AC5" r:id="rId8" xr:uid="{5ED3647C-C8FA-443D-AAEB-9454BBCF6176}"/>
+    <hyperlink ref="AC4" r:id="rId9" xr:uid="{118612AF-F178-449D-94F5-EA8FCCE6B629}"/>
+    <hyperlink ref="AC6" r:id="rId10" xr:uid="{9F819B38-1C37-4436-86A4-26447E432B97}"/>
+    <hyperlink ref="AC8" r:id="rId11" xr:uid="{3E18BD0A-C819-47DD-AF95-3DFEF2DEB3D5}"/>
+    <hyperlink ref="AC11" r:id="rId12" xr:uid="{E2C80B92-5270-44E6-BA42-98A672C126C8}"/>
+    <hyperlink ref="AC9" r:id="rId13" xr:uid="{65DBFE01-0236-40D1-BAA2-DBC7A7D06BBE}"/>
+    <hyperlink ref="AC7" r:id="rId14" xr:uid="{31303705-0E07-4F0C-A889-CB48F2A8D49E}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId15"/>
@@ -1480,6 +1523,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100886399F21440F54B81A4893F74DA4F94" ma:contentTypeVersion="8" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="91b6ab92f34ab688a19900d483ae7505">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0190bee1-42b9-4362-9dc8-2229f310bd34" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d4f82e64d1772ab8a19658e1978de7e8" ns3:_="">
     <xsd:import namespace="0190bee1-42b9-4362-9dc8-2229f310bd34"/>
@@ -1649,15 +1701,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1665,6 +1708,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6C04E1C-86C9-4DFF-AFD3-8243B20410CC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FBDDB8E-E50B-4DEA-B8C8-CD7F650AB124}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1678,14 +1729,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6C04E1C-86C9-4DFF-AFD3-8243B20410CC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Inclusão do Modelo T5 em inglês e português.
</commit_message>
<xml_diff>
--- a/modelos.xlsx
+++ b/modelos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\osmar\Documentos\GitHub\texto-transformer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E28F0E42-1902-4C86-89EC-9955FC61A812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B46412-A73A-427B-B976-76481D1DDF5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{ADA84CBB-E06D-42EE-8062-4654A38564A2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="114">
   <si>
     <t>modelo</t>
   </si>
@@ -296,9 +296,6 @@
     <t>Posição do primeiro token válido</t>
   </si>
   <si>
-    <t>Posição do último token válido</t>
-  </si>
-  <si>
     <t>['&lt;s&gt;', '▁Fresh', '▁sea', '▁bas', 's', '▁is', '▁a', '▁great', '▁de', 'lica', 'cy', '.', '&lt;/s&gt;']</t>
   </si>
   <si>
@@ -351,6 +348,36 @@
   </si>
   <si>
     <t>Nomes huggingface</t>
+  </si>
+  <si>
+    <t>T5</t>
+  </si>
+  <si>
+    <t>&lt;extra_id_0&gt;</t>
+  </si>
+  <si>
+    <t>X &lt;/s&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A &lt;/s&gt; B &lt;/s&gt; </t>
+  </si>
+  <si>
+    <t>https://huggingface.co/docs/transformers/model_doc/t5#transformers.T5Tokenizer</t>
+  </si>
+  <si>
+    <t>https://github.com/huggingface/transformers/blob/v4.34.0/src/transformers/models/t5/tokenization_t5.py#L63</t>
+  </si>
+  <si>
+    <t>Posição do último token válido (-1 - ultimo, -2 penúltimo)</t>
+  </si>
+  <si>
+    <t>['▁Fresh', '▁sea', '▁bass', '▁is', 'a', '▁great', '▁de', 'lic', 'acy', '.', '&lt;/s&gt;']</t>
+  </si>
+  <si>
+    <t>Não é o caracter _ simples é o caracter â–.</t>
+  </si>
+  <si>
+    <t>Obs.</t>
   </si>
 </sst>
 </file>
@@ -742,10 +769,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D3D3DC9-8A8A-4ECE-AF2B-5AE8D9558D5B}">
-  <dimension ref="A2:AC23"/>
+  <dimension ref="A2:AD24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -759,16 +786,16 @@
     <col min="7" max="7" width="6.140625" customWidth="1"/>
     <col min="8" max="8" width="8" customWidth="1"/>
     <col min="9" max="9" width="7.5703125" customWidth="1"/>
-    <col min="10" max="15" width="5.5703125" customWidth="1"/>
-    <col min="16" max="16" width="6.140625" customWidth="1"/>
-    <col min="18" max="18" width="13" customWidth="1"/>
-    <col min="19" max="19" width="20" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="16" width="5.5703125" customWidth="1"/>
+    <col min="17" max="17" width="6.140625" customWidth="1"/>
+    <col min="19" max="19" width="13" customWidth="1"/>
+    <col min="20" max="20" width="20" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>28</v>
@@ -800,85 +827,89 @@
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
-      <c r="P2" s="2" t="s">
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
-      <c r="AB2" s="1" t="s">
+      <c r="U2" s="2"/>
+      <c r="AC2" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AD2" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="K3" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="M3" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="J3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="M3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="P3" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="Q3" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="P3" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q3" s="2" t="s">
+      <c r="R3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="R3" s="2" t="s">
+      <c r="S3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="S3" s="2" t="s">
+      <c r="T3" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="T3" s="2" t="s">
+      <c r="U3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="AB3" s="1"/>
       <c r="AC3" s="1"/>
-    </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD3" s="1"/>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -909,44 +940,47 @@
       <c r="J4" t="s">
         <v>5</v>
       </c>
-      <c r="K4">
-        <v>1</v>
+      <c r="K4" t="s">
+        <v>112</v>
       </c>
       <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
         <v>-1</v>
       </c>
-      <c r="M4">
-        <v>1</v>
-      </c>
       <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4">
         <v>0</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>9</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>13</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>41</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
         <v>42</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>53</v>
       </c>
-      <c r="AB4" s="4" t="s">
+      <c r="AC4" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="AC4" s="4" t="s">
+      <c r="AD4" s="4" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -977,44 +1011,44 @@
       <c r="J5" t="s">
         <v>4</v>
       </c>
-      <c r="K5">
-        <v>1</v>
-      </c>
       <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
         <v>-1</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
       </c>
       <c r="N5">
         <v>0</v>
       </c>
-      <c r="O5" t="s">
-        <v>9</v>
+      <c r="O5">
+        <v>0</v>
       </c>
       <c r="P5" t="s">
         <v>9</v>
       </c>
       <c r="Q5" t="s">
+        <v>9</v>
+      </c>
+      <c r="R5" t="s">
         <v>15</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>41</v>
       </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
         <v>42</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>51</v>
       </c>
-      <c r="AB5" s="4" t="s">
+      <c r="AC5" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="AC5" s="4" t="s">
+      <c r="AD5" s="4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1045,46 +1079,46 @@
       <c r="J6" t="s">
         <v>4</v>
       </c>
-      <c r="K6">
-        <v>1</v>
-      </c>
       <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
         <v>-1</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
       </c>
       <c r="N6">
         <v>0</v>
       </c>
-      <c r="O6" t="s">
-        <v>9</v>
+      <c r="O6">
+        <v>0</v>
       </c>
       <c r="P6" t="s">
         <v>9</v>
       </c>
       <c r="Q6" t="s">
+        <v>9</v>
+      </c>
+      <c r="R6" t="s">
         <v>12</v>
       </c>
-      <c r="R6" t="s">
+      <c r="S6" t="s">
         <v>41</v>
       </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
         <v>42</v>
       </c>
-      <c r="T6" t="s">
+      <c r="U6" t="s">
         <v>51</v>
       </c>
-      <c r="AB6" s="4" t="s">
+      <c r="AC6" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="AC6" s="4" t="s">
+      <c r="AD6" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>46</v>
@@ -1113,44 +1147,44 @@
       <c r="J7" t="s">
         <v>6</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>0</v>
       </c>
-      <c r="L7" s="5" t="s">
+      <c r="M7" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="M7">
-        <v>1</v>
-      </c>
       <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
         <v>0</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>7</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>9</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="R7" t="s">
         <v>14</v>
       </c>
-      <c r="R7" t="s">
+      <c r="S7" t="s">
         <v>47</v>
       </c>
-      <c r="S7" t="s">
+      <c r="T7" t="s">
         <v>48</v>
       </c>
-      <c r="T7" t="s">
+      <c r="U7" t="s">
         <v>52</v>
       </c>
-      <c r="AB7" s="4" t="s">
+      <c r="AC7" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="AC7" s="4" t="s">
+      <c r="AD7" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -1181,44 +1215,44 @@
       <c r="J8" t="s">
         <v>6</v>
       </c>
-      <c r="K8">
-        <v>1</v>
-      </c>
       <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
         <v>-1</v>
       </c>
-      <c r="M8">
-        <v>1</v>
-      </c>
       <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8">
         <v>0</v>
       </c>
-      <c r="O8" t="s">
+      <c r="P8" t="s">
         <v>7</v>
       </c>
-      <c r="P8" t="s">
+      <c r="Q8" t="s">
         <v>9</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="R8" t="s">
         <v>14</v>
       </c>
-      <c r="R8" t="s">
+      <c r="S8" t="s">
         <v>40</v>
       </c>
-      <c r="S8" t="s">
+      <c r="T8" t="s">
         <v>84</v>
       </c>
-      <c r="T8" t="s">
+      <c r="U8" t="s">
         <v>60</v>
       </c>
-      <c r="AB8" s="4" t="s">
+      <c r="AC8" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="AC8" s="4" t="s">
+      <c r="AD8" s="4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>49</v>
       </c>
@@ -1249,44 +1283,44 @@
       <c r="J9" t="s">
         <v>50</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>0</v>
       </c>
-      <c r="L9" s="5" t="s">
+      <c r="M9" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>2</v>
       </c>
-      <c r="N9">
-        <v>1</v>
-      </c>
-      <c r="O9" t="s">
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="P9" t="s">
         <v>9</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" t="s">
         <v>7</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="R9" t="s">
         <v>14</v>
       </c>
-      <c r="R9" t="s">
+      <c r="S9" t="s">
         <v>47</v>
       </c>
-      <c r="S9" t="s">
+      <c r="T9" t="s">
         <v>48</v>
       </c>
-      <c r="T9" t="s">
+      <c r="U9" t="s">
         <v>55</v>
       </c>
-      <c r="AB9" s="4" t="s">
+      <c r="AC9" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="AC9" s="4" t="s">
+      <c r="AD9" s="4" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>81</v>
       </c>
@@ -1317,44 +1351,47 @@
       <c r="J10" t="s">
         <v>5</v>
       </c>
-      <c r="K10">
-        <v>1</v>
+      <c r="K10" t="s">
+        <v>112</v>
       </c>
       <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10">
         <v>-1</v>
       </c>
-      <c r="M10">
-        <v>1</v>
-      </c>
       <c r="N10">
+        <v>1</v>
+      </c>
+      <c r="O10">
         <v>0</v>
-      </c>
-      <c r="O10" t="s">
-        <v>9</v>
       </c>
       <c r="P10" t="s">
         <v>9</v>
       </c>
       <c r="Q10" t="s">
+        <v>9</v>
+      </c>
+      <c r="R10" t="s">
         <v>13</v>
       </c>
-      <c r="R10" t="s">
+      <c r="S10" t="s">
         <v>40</v>
       </c>
-      <c r="S10" t="s">
+      <c r="T10" t="s">
         <v>84</v>
       </c>
-      <c r="T10" t="s">
-        <v>87</v>
-      </c>
-      <c r="AB10" s="4" t="s">
+      <c r="U10" t="s">
+        <v>86</v>
+      </c>
+      <c r="AC10" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="AC10" s="4" t="s">
+      <c r="AD10" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -1385,137 +1422,211 @@
       <c r="J11" t="s">
         <v>5</v>
       </c>
-      <c r="K11">
+      <c r="K11" t="s">
+        <v>112</v>
+      </c>
+      <c r="L11">
         <v>0</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <v>-2</v>
       </c>
-      <c r="M11">
-        <v>1</v>
-      </c>
       <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="O11">
         <v>0</v>
-      </c>
-      <c r="O11" t="s">
-        <v>9</v>
       </c>
       <c r="P11" t="s">
         <v>9</v>
       </c>
       <c r="Q11" t="s">
+        <v>9</v>
+      </c>
+      <c r="R11" t="s">
         <v>13</v>
       </c>
-      <c r="R11" t="s">
+      <c r="S11" t="s">
         <v>43</v>
       </c>
-      <c r="S11" t="s">
+      <c r="T11" t="s">
         <v>44</v>
       </c>
-      <c r="T11" t="s">
+      <c r="U11" t="s">
         <v>54</v>
       </c>
-      <c r="AB11" s="4" t="s">
+      <c r="AC11" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="AC11" s="4" t="s">
+      <c r="AD11" s="4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="M13">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12" t="s">
+        <v>105</v>
+      </c>
+      <c r="I12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J12" t="s">
+        <v>5</v>
+      </c>
+      <c r="K12" t="s">
+        <v>112</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
         <v>-1</v>
       </c>
-      <c r="N13" t="s">
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>9</v>
+      </c>
+      <c r="R12" t="s">
+        <v>13</v>
+      </c>
+      <c r="S12" t="s">
+        <v>106</v>
+      </c>
+      <c r="T12" t="s">
+        <v>107</v>
+      </c>
+      <c r="U12" t="s">
+        <v>111</v>
+      </c>
+      <c r="AC12" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="AD12" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="N14">
+        <v>-1</v>
+      </c>
+      <c r="O14" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="G14">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="G15">
         <v>0</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H15" t="s">
         <v>79</v>
       </c>
-      <c r="M14">
+      <c r="N15">
         <v>0</v>
       </c>
-      <c r="N14" t="s">
+      <c r="O15" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="G15">
-        <v>1</v>
-      </c>
-      <c r="H15" t="s">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16" t="s">
         <v>80</v>
       </c>
-      <c r="M15">
-        <v>1</v>
-      </c>
-      <c r="N15" t="s">
+      <c r="N16">
+        <v>1</v>
+      </c>
+      <c r="O16" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="M16">
+    <row r="17" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="N17">
         <v>2</v>
       </c>
-      <c r="N16" t="s">
+      <c r="O17" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="11:15" x14ac:dyDescent="0.25">
-      <c r="K18" t="s">
+    <row r="19" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L19" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="11:15" x14ac:dyDescent="0.25">
-      <c r="L19" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="21" spans="11:15" x14ac:dyDescent="0.25">
-      <c r="N21">
+    <row r="20" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="M20" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="O22">
         <v>-1</v>
       </c>
-      <c r="O21" t="s">
+      <c r="P22" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="11:15" x14ac:dyDescent="0.25">
-      <c r="N22">
+    <row r="23" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="O23">
         <v>0</v>
       </c>
-      <c r="O22" t="s">
+      <c r="P23" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="11:15" x14ac:dyDescent="0.25">
-      <c r="N23">
-        <v>1</v>
-      </c>
-      <c r="O23" t="s">
+    <row r="24" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="O24">
+        <v>1</v>
+      </c>
+      <c r="P24" t="s">
         <v>57</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="AB5" r:id="rId1" location="transformers.BertTokenizer" xr:uid="{34D2F53E-DD38-4D02-B9D7-EEB3C73565A4}"/>
-    <hyperlink ref="AB4" r:id="rId2" location="transformers.AlbertTokenizer" xr:uid="{1C747986-9A2C-4D37-85D4-551E037E79AF}"/>
-    <hyperlink ref="AB6" r:id="rId3" location="transformers.DistilBertTokenizer" xr:uid="{4557F4E1-3CF5-452D-B493-FBA68FEF70C1}"/>
-    <hyperlink ref="AB8" r:id="rId4" location="transformers.RobertaTokenizer" xr:uid="{38642F05-9C73-4563-BF96-AEE8C072DC8E}"/>
-    <hyperlink ref="AB11" r:id="rId5" location="transformers.XLNetTokenizer" xr:uid="{287DC99E-D4A0-4091-81B9-FD3CC7A6D5AB}"/>
-    <hyperlink ref="AB9" r:id="rId6" location="transformers.OpenAIGPTTokenizer" xr:uid="{1381AF7A-FED8-43A8-B952-743B3E821ABF}"/>
-    <hyperlink ref="AB7" r:id="rId7" location="transformers.GPT2Tokenizer" xr:uid="{D91A5263-1AFB-40F8-BF67-C0F7CF6DD3B8}"/>
-    <hyperlink ref="AC5" r:id="rId8" xr:uid="{5ED3647C-C8FA-443D-AAEB-9454BBCF6176}"/>
-    <hyperlink ref="AC4" r:id="rId9" xr:uid="{118612AF-F178-449D-94F5-EA8FCCE6B629}"/>
-    <hyperlink ref="AC6" r:id="rId10" xr:uid="{9F819B38-1C37-4436-86A4-26447E432B97}"/>
-    <hyperlink ref="AC8" r:id="rId11" xr:uid="{3E18BD0A-C819-47DD-AF95-3DFEF2DEB3D5}"/>
-    <hyperlink ref="AC11" r:id="rId12" xr:uid="{E2C80B92-5270-44E6-BA42-98A672C126C8}"/>
-    <hyperlink ref="AC9" r:id="rId13" xr:uid="{65DBFE01-0236-40D1-BAA2-DBC7A7D06BBE}"/>
-    <hyperlink ref="AC7" r:id="rId14" xr:uid="{31303705-0E07-4F0C-A889-CB48F2A8D49E}"/>
+    <hyperlink ref="AC5" r:id="rId1" location="transformers.BertTokenizer" xr:uid="{34D2F53E-DD38-4D02-B9D7-EEB3C73565A4}"/>
+    <hyperlink ref="AC4" r:id="rId2" location="transformers.AlbertTokenizer" xr:uid="{1C747986-9A2C-4D37-85D4-551E037E79AF}"/>
+    <hyperlink ref="AC6" r:id="rId3" location="transformers.DistilBertTokenizer" xr:uid="{4557F4E1-3CF5-452D-B493-FBA68FEF70C1}"/>
+    <hyperlink ref="AC8" r:id="rId4" location="transformers.RobertaTokenizer" xr:uid="{38642F05-9C73-4563-BF96-AEE8C072DC8E}"/>
+    <hyperlink ref="AC11" r:id="rId5" location="transformers.XLNetTokenizer" xr:uid="{287DC99E-D4A0-4091-81B9-FD3CC7A6D5AB}"/>
+    <hyperlink ref="AC9" r:id="rId6" location="transformers.OpenAIGPTTokenizer" xr:uid="{1381AF7A-FED8-43A8-B952-743B3E821ABF}"/>
+    <hyperlink ref="AC7" r:id="rId7" location="transformers.GPT2Tokenizer" xr:uid="{D91A5263-1AFB-40F8-BF67-C0F7CF6DD3B8}"/>
+    <hyperlink ref="AD5" r:id="rId8" xr:uid="{5ED3647C-C8FA-443D-AAEB-9454BBCF6176}"/>
+    <hyperlink ref="AD4" r:id="rId9" xr:uid="{118612AF-F178-449D-94F5-EA8FCCE6B629}"/>
+    <hyperlink ref="AD6" r:id="rId10" xr:uid="{9F819B38-1C37-4436-86A4-26447E432B97}"/>
+    <hyperlink ref="AD8" r:id="rId11" xr:uid="{3E18BD0A-C819-47DD-AF95-3DFEF2DEB3D5}"/>
+    <hyperlink ref="AD11" r:id="rId12" xr:uid="{E2C80B92-5270-44E6-BA42-98A672C126C8}"/>
+    <hyperlink ref="AD9" r:id="rId13" xr:uid="{65DBFE01-0236-40D1-BAA2-DBC7A7D06BBE}"/>
+    <hyperlink ref="AD7" r:id="rId14" xr:uid="{31303705-0E07-4F0C-A889-CB48F2A8D49E}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId15"/>

</xml_diff>